<commit_message>
Mise à jour du journal de travail
</commit_message>
<xml_diff>
--- a/Documentation/Journaux/Joao-JournalDeTravail.xlsx
+++ b/Documentation/Journaux/Joao-JournalDeTravail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CPNV\2emeAnnee\2emeSemestre\MA\Projet-WEB\Mouse-to-House-BDD\Documentation\Journaux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D0BF2C-194A-4EDC-89DD-8EAAEB3CD6BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F4DD536-EEED-4AF6-8B64-90C659067A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -85,19 +85,28 @@
     <t>M. Hurni nous a expliqué GitHub</t>
   </si>
   <si>
-    <t>Création des différentes features du projet</t>
-  </si>
-  <si>
-    <t>Ajout de quelques tâches au premier sprint</t>
-  </si>
-  <si>
     <t>Icesrum</t>
   </si>
   <si>
     <t>MCD</t>
   </si>
   <si>
-    <t>Finalization du MCD</t>
+    <t>MLD</t>
+  </si>
+  <si>
+    <t>J'ai commencé le MLD</t>
+  </si>
+  <si>
+    <t>J'ai finalizé le MCD</t>
+  </si>
+  <si>
+    <t>J'ai ajouté quelques tâches au premier sprint</t>
+  </si>
+  <si>
+    <t>J'ai créé les différentes features du projet</t>
+  </si>
+  <si>
+    <t>J'ai continué le MLD</t>
   </si>
 </sst>
 </file>
@@ -465,8 +474,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau4" displayName="Tableau4" ref="A1:H9" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9">
-  <autoFilter ref="A1:H9" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau4" displayName="Tableau4" ref="A1:H11" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9">
+  <autoFilter ref="A1:H11" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Heure début" dataDxfId="6"/>
@@ -746,10 +755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -907,10 +916,10 @@
         <v>8</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="H6" s="7"/>
     </row>
@@ -932,10 +941,10 @@
         <v>8</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H7" s="7"/>
     </row>
@@ -957,10 +966,10 @@
         <v>8</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H8" s="7"/>
     </row>
@@ -982,12 +991,62 @@
         <v>8</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>20</v>
       </c>
       <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="9">
+        <v>45050</v>
+      </c>
+      <c r="B10" s="12">
+        <v>0.56527777777777777</v>
+      </c>
+      <c r="C10" s="12">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="D10" s="8">
+        <f>Tableau4[[#This Row],[Heure fin]]-Tableau4[[#This Row],[Heure début]]</f>
+        <v>6.3194444444444442E-2</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="9">
+        <v>45050</v>
+      </c>
+      <c r="B11" s="12">
+        <v>0.64097222222222217</v>
+      </c>
+      <c r="C11" s="12">
+        <v>0.66597222222222219</v>
+      </c>
+      <c r="D11" s="8">
+        <f>Tableau4[[#This Row],[Heure fin]]-Tableau4[[#This Row],[Heure début]]</f>
+        <v>2.5000000000000022E-2</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="7"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">

</xml_diff>

<commit_message>
debut script base de donnees
</commit_message>
<xml_diff>
--- a/Documentation/Journaux/Joao-JournalDeTravail.xlsx
+++ b/Documentation/Journaux/Joao-JournalDeTravail.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joao-Alexandre.CARVA\Documents\GitHub\Mouse-to-House-BDD\Documentation\Journaux\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjetWeb\Mouse-to-House-BDD\Documentation\Journaux\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -109,6 +109,18 @@
   </si>
   <si>
     <t>J'ai fini le MLD</t>
+  </si>
+  <si>
+    <t>Cahier des Charges</t>
+  </si>
+  <si>
+    <t>J'ai fait une mise en comum du cahier des charges avec Evann</t>
+  </si>
+  <si>
+    <t>Base de données</t>
+  </si>
+  <si>
+    <t>J'ai commencé le script pour créer la base de données</t>
   </si>
 </sst>
 </file>
@@ -488,8 +500,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="A1:H13" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12">
-  <autoFilter ref="A1:H13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="A1:H14" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12">
+  <autoFilter ref="A1:H14"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Date" dataDxfId="10"/>
     <tableColumn id="2" name="Heure début" dataDxfId="9"/>
@@ -769,10 +781,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,7 +849,7 @@
       </c>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>45042</v>
       </c>
@@ -1094,15 +1106,48 @@
       <c r="B13" s="15">
         <v>0.37916666666666665</v>
       </c>
-      <c r="C13" s="15"/>
+      <c r="C13" s="15">
+        <v>0.39861111111111108</v>
+      </c>
       <c r="D13" s="16">
         <f>Tableau4[[#This Row],[Heure fin]]-Tableau4[[#This Row],[Heure début]]</f>
-        <v>-0.37916666666666665</v>
-      </c>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
+        <v>1.9444444444444431E-2</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>26</v>
+      </c>
       <c r="H13" s="17"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="14">
+        <v>45056</v>
+      </c>
+      <c r="B14" s="15">
+        <v>0.64097222222222217</v>
+      </c>
+      <c r="C14" s="15">
+        <v>0.70277777777777783</v>
+      </c>
+      <c r="D14" s="16">
+        <f>Tableau4[[#This Row],[Heure fin]]-Tableau4[[#This Row],[Heure début]]</f>
+        <v>6.1805555555555669E-2</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="17"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">

</xml_diff>

<commit_message>
Backup de la base de données fait
</commit_message>
<xml_diff>
--- a/Documentation/Journaux/Joao-JournalDeTravail.xlsx
+++ b/Documentation/Journaux/Joao-JournalDeTravail.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -121,6 +121,15 @@
   </si>
   <si>
     <t>J'ai commencé le script pour créer la base de données</t>
+  </si>
+  <si>
+    <t>M. Meylan</t>
+  </si>
+  <si>
+    <t>J'ai fini le scriptqui crée la base de données</t>
+  </si>
+  <si>
+    <t>J'ai fait un script qui crée un backup de la base de données</t>
   </si>
 </sst>
 </file>
@@ -500,8 +509,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="A1:H14" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12">
-  <autoFilter ref="A1:H14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="A1:H16" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12">
+  <autoFilter ref="A1:H16"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Date" dataDxfId="10"/>
     <tableColumn id="2" name="Heure début" dataDxfId="9"/>
@@ -781,10 +790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1148,6 +1157,58 @@
         <v>28</v>
       </c>
       <c r="H14" s="17"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="14">
+        <v>45057</v>
+      </c>
+      <c r="B15" s="15">
+        <v>0.56527777777777777</v>
+      </c>
+      <c r="C15" s="15">
+        <v>0.65208333333333335</v>
+      </c>
+      <c r="D15" s="16">
+        <f>Tableau4[[#This Row],[Heure fin]]-Tableau4[[#This Row],[Heure début]]</f>
+        <v>8.680555555555558E-2</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="14">
+        <v>45057</v>
+      </c>
+      <c r="B16" s="15">
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="C16" s="15">
+        <v>0.66041666666666665</v>
+      </c>
+      <c r="D16" s="16">
+        <f>Tableau4[[#This Row],[Heure fin]]-Tableau4[[#This Row],[Heure début]]</f>
+        <v>7.6388888888888618E-3</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16" s="17"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">

</xml_diff>

<commit_message>
Début de l'ajout des produits à la base de données
</commit_message>
<xml_diff>
--- a/Documentation/Journaux/Joao-JournalDeTravail.xlsx
+++ b/Documentation/Journaux/Joao-JournalDeTravail.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -126,10 +126,16 @@
     <t>M. Meylan</t>
   </si>
   <si>
-    <t>J'ai fini le scriptqui crée la base de données</t>
-  </si>
-  <si>
     <t>J'ai fait un script qui crée un backup de la base de données</t>
+  </si>
+  <si>
+    <t>J'ai fini le script qui crée la base de données</t>
+  </si>
+  <si>
+    <t>J'ai commencé le script qui ajoutera tous les produits à la base de données</t>
+  </si>
+  <si>
+    <t>M. Hurni</t>
   </si>
 </sst>
 </file>
@@ -509,8 +515,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="A1:H16" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12">
-  <autoFilter ref="A1:H16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="A1:H17" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12">
+  <autoFilter ref="A1:H17"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Date" dataDxfId="10"/>
     <tableColumn id="2" name="Heure début" dataDxfId="9"/>
@@ -790,10 +796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,7 +1185,7 @@
         <v>27</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H15" s="17" t="s">
         <v>29</v>
@@ -1206,9 +1212,36 @@
         <v>27</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H16" s="17"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="14">
+        <v>45061</v>
+      </c>
+      <c r="B17" s="15">
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="C17" s="15">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D17" s="16">
+        <f>Tableau4[[#This Row],[Heure fin]]-Tableau4[[#This Row],[Heure début]]</f>
+        <v>5.9027777777777735E-2</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" s="17" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">

</xml_diff>